<commit_message>
fix: update template file in storage
</commit_message>
<xml_diff>
--- a/storage/app/public/templates/6xGSAprFh0YgkReR9xCUt9xvKKyXMzv1bQ83IGNy.xlsx
+++ b/storage/app/public/templates/6xGSAprFh0YgkReR9xCUt9xvKKyXMzv1bQ83IGNy.xlsx
@@ -1,17 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10526"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F01A9C-5FD4-8A4B-A765-F89F1B418CE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="22540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Rekap nilai" state="visible" r:id="rId4"/>
+    <sheet name="Rekap nilai" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="101">
   <si>
     <t>Niplama</t>
   </si>
@@ -311,24 +315,32 @@
   </si>
   <si>
     <t>Kepala Subbagian Umum</t>
+  </si>
+  <si>
+    <t>Butir</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
-    <font/>
   </fonts>
   <fills count="3">
     <fill>
@@ -339,7 +351,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="C6E0B4"/>
+        <fgColor rgb="FFC6E0B4"/>
       </patternFill>
     </fill>
   </fills>
@@ -352,10 +364,18 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -364,7 +384,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -706,9 +726,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J29"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
@@ -716,9 +741,10 @@
     <col min="4" max="4" width="30" customWidth="1"/>
     <col min="5" max="9" width="20" customWidth="1"/>
     <col min="10" max="10" width="15" customWidth="1"/>
+    <col min="11" max="11" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -749,8 +775,11 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -781,8 +810,9 @@
       <c r="J2" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>20</v>
       </c>
@@ -813,8 +843,9 @@
       <c r="J3" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>24</v>
       </c>
@@ -845,8 +876,9 @@
       <c r="J4" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>26</v>
       </c>
@@ -877,8 +909,9 @@
       <c r="J5" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>31</v>
       </c>
@@ -909,8 +942,9 @@
       <c r="J6" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>37</v>
       </c>
@@ -941,8 +975,9 @@
       <c r="J7" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>40</v>
       </c>
@@ -973,8 +1008,9 @@
       <c r="J8" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>42</v>
       </c>
@@ -1005,8 +1041,9 @@
       <c r="J9" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>47</v>
       </c>
@@ -1037,8 +1074,9 @@
       <c r="J10" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>49</v>
       </c>
@@ -1069,8 +1107,9 @@
       <c r="J11" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>51</v>
       </c>
@@ -1101,8 +1140,9 @@
       <c r="J12" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>53</v>
       </c>
@@ -1133,8 +1173,9 @@
       <c r="J13" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>55</v>
       </c>
@@ -1165,8 +1206,9 @@
       <c r="J14" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>57</v>
       </c>
@@ -1197,8 +1239,9 @@
       <c r="J15" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>61</v>
       </c>
@@ -1229,8 +1272,9 @@
       <c r="J16" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>66</v>
       </c>
@@ -1261,8 +1305,9 @@
       <c r="J17" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>69</v>
       </c>
@@ -1293,8 +1338,9 @@
       <c r="J18" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>71</v>
       </c>
@@ -1325,8 +1371,9 @@
       <c r="J19" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>73</v>
       </c>
@@ -1357,8 +1404,9 @@
       <c r="J20" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>76</v>
       </c>
@@ -1389,8 +1437,9 @@
       <c r="J21" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>79</v>
       </c>
@@ -1421,8 +1470,9 @@
       <c r="J22" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K22" s="2"/>
+    </row>
+    <row r="23" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>82</v>
       </c>
@@ -1453,8 +1503,9 @@
       <c r="J23" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K23" s="2"/>
+    </row>
+    <row r="24" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>84</v>
       </c>
@@ -1485,8 +1536,9 @@
       <c r="J24" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K24" s="2"/>
+    </row>
+    <row r="25" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>87</v>
       </c>
@@ -1517,8 +1569,9 @@
       <c r="J25" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K25" s="2"/>
+    </row>
+    <row r="26" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>89</v>
       </c>
@@ -1549,8 +1602,9 @@
       <c r="J26" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K26" s="2"/>
+    </row>
+    <row r="27" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>91</v>
       </c>
@@ -1581,8 +1635,9 @@
       <c r="J27" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K27" s="2"/>
+    </row>
+    <row r="28" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>93</v>
       </c>
@@ -1613,8 +1668,9 @@
       <c r="J28" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K28" s="2"/>
+    </row>
+    <row r="29" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>97</v>
       </c>
@@ -1645,9 +1701,10 @@
       <c r="J29" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="K29" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>